<commit_message>
Bài 29 - DataProvider in TestNG and read data from Excel
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/LoginData.xlsx
+++ b/src/test/resources/testdata/LoginData.xlsx
@@ -8,16 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ANHTESTER\SeleniumJava\ViettelAutoTest\Viettel_SeleniumTestNG_Parallel\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22882464-8535-4F75-8109-85A3CF6A7789}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FBC022C-7ABA-4304-BF82-88AF222A6936}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4788" yWindow="1644" windowWidth="22704" windowHeight="13872" xr2:uid="{A9ACE44C-53B5-4123-811A-ADDB2C6358BA}"/>
+    <workbookView xWindow="7056" yWindow="1740" windowWidth="22704" windowHeight="13872" xr2:uid="{A9ACE44C-53B5-4123-811A-ADDB2C6358BA}"/>
   </bookViews>
   <sheets>
-    <sheet name="LoginSuccess" sheetId="1" r:id="rId1"/>
-    <sheet name="LoginFail" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
-    <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
+    <sheet name="LoginData" sheetId="6" r:id="rId1"/>
+    <sheet name="LoginSuccess" sheetId="1" r:id="rId2"/>
+    <sheet name="LoginFail" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
   <si>
     <t>email</t>
   </si>
@@ -76,6 +74,12 @@
   </si>
   <si>
     <t>project manager</t>
+  </si>
+  <si>
+    <t>1234567</t>
+  </si>
+  <si>
+    <t>employee@example.com</t>
   </si>
 </sst>
 </file>
@@ -125,12 +129,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -445,11 +450,67 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7D41B7A-CB75-4950-A398-E0E48FF98C84}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="24.15234375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{3CEA9081-9F48-400A-9DB2-F998BDB61307}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{B280CB87-4F49-4A13-A2EA-A7C263723546}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{920E2C0D-F901-4A8E-95ED-33B920E317B0}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{702E0357-99BA-421C-B65D-B7218FD89C6B}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD10"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.3"/>
@@ -508,7 +569,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A863FC0-C8AF-46C3-91C4-009D49638BAD}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -549,40 +610,4 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FE85D7A-4768-41C0-8A45-8E3FBEE50113}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13FA9F59-8C50-40B0-916D-2598D476866A}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A52E0180-C0DE-45AC-8AB4-8D643CAF9397}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>